<commit_message>
1. Reduced num-boosters to complete benchmarking in reasonable time 2. Updated benchmark numbers after fixing an issue with xgboost benchmark code
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="950" yWindow="0" windowWidth="27860" windowHeight="14240" xr2:uid="{C0E4B2E6-10A6-4D57-86C8-635D3547ADB2}"/>
+    <workbookView xWindow="1890" yWindow="0" windowWidth="27855" windowHeight="14235" xr2:uid="{C0E4B2E6-10A6-4D57-86C8-635D3547ADB2}"/>
   </bookViews>
   <sheets>
-    <sheet name="21.11.2017" sheetId="1" r:id="rId1"/>
+    <sheet name="28.11.2017" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="39">
   <si>
     <t>airline</t>
   </si>
@@ -122,13 +122,25 @@
     <t>model name      : Intel(R) Xeon(R) CPU E5-2698 v3 @ 2.30GHz</t>
   </si>
   <si>
-    <t>GPU 0: Tesla P100-PCIE-16GB (UUID: GPU-74dff14b-a797-85d9-b64a-5293c94557a6)</t>
-  </si>
-  <si>
-    <t>Description:    CentOS Linux release 7.3.1611 (Core)</t>
-  </si>
-  <si>
     <t>| NVIDIA-SMI 384.81                 Driver Version: 384.81                    |</t>
+  </si>
+  <si>
+    <t>GPU 0: Tesla P100-PCIE-16GB (UUID: GPU-60a2589c-3815-802f-3553-c649e6a332f4)</t>
+  </si>
+  <si>
+    <t>Linux de283d05c594 3.10.0-514.21.1.el7.x86_64 #1 SMP Thu May 25 17:04:51 UTC 2017 x86_64 x86_64 x86_64 GNU/Linux</t>
+  </si>
+  <si>
+    <t>XGBoost  Commit: 77ae4c870178be3c4dbe5331ec7966cec93fee33</t>
+  </si>
+  <si>
+    <t>LightGBM Commit: 04d4811b4e6d51542bd2e2e23d0e608a9732ea30</t>
+  </si>
+  <si>
+    <t>CatBoost Commit: f28154d8b0d4ca8e4d1baed2260656ba1223a75d</t>
+  </si>
+  <si>
+    <t>seconds</t>
   </si>
 </sst>
 </file>
@@ -493,18 +505,24 @@
   <dimension ref="A1:P73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+      <selection activeCell="Q29" sqref="Q29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="8" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.54296875" customWidth="1"/>
-    <col min="11" max="11" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.5703125" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="J1" s="1" t="s">
         <v>25</v>
       </c>
@@ -515,7 +533,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -544,252 +562,261 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3">
-        <v>705.78660488128605</v>
+        <v>327.85048413276598</v>
       </c>
       <c r="C3">
-        <v>8.4927918910980207</v>
+        <v>6.9443659782409597</v>
       </c>
       <c r="D3">
-        <v>0.74122996684998499</v>
+        <v>0.72115824186937105</v>
       </c>
       <c r="E3">
-        <v>0.74083449999999995</v>
+        <v>0.72141100000000002</v>
       </c>
       <c r="F3">
-        <v>0.747905866491967</v>
+        <v>0.73221865508093298</v>
       </c>
       <c r="G3">
-        <v>0.76329728224532301</v>
+        <v>0.73819346967530497</v>
       </c>
       <c r="H3">
-        <v>0.73312289845205902</v>
+        <v>0.72633978225186302</v>
       </c>
       <c r="J3" t="s">
         <v>26</v>
       </c>
       <c r="K3">
         <f>B3/B4</f>
-        <v>4.356966729022302</v>
+        <v>3.2368926781584051</v>
       </c>
       <c r="P3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4">
-        <v>161.99035906791599</v>
+        <v>101.28555893898</v>
       </c>
       <c r="C4">
-        <v>8.5367159843444806</v>
+        <v>7.2891988754272399</v>
       </c>
       <c r="D4">
-        <v>0.74250390067162797</v>
+        <v>0.72590733526718398</v>
       </c>
       <c r="E4">
-        <v>0.74206649999999996</v>
+        <v>0.72586649999999997</v>
       </c>
       <c r="F4">
-        <v>0.74890947020841003</v>
+        <v>0.73502739777666704</v>
       </c>
       <c r="G4">
-        <v>0.76493983696346501</v>
+        <v>0.74526186939875905</v>
       </c>
       <c r="H4">
-        <v>0.73353718914491595</v>
+        <v>0.72507021249918302</v>
       </c>
       <c r="J4" t="s">
         <v>27</v>
       </c>
       <c r="K4">
         <f>B5/B6</f>
-        <v>1.2066171227196598</v>
+        <v>1.2499499969943728</v>
       </c>
       <c r="P4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5">
-        <v>165.82736301422099</v>
+        <v>84.521354913711505</v>
       </c>
       <c r="C5">
-        <v>6.3640818595886204</v>
+        <v>3.3380930423736501</v>
       </c>
       <c r="D5">
-        <v>0.88066234433784796</v>
+        <v>0.86444707500946805</v>
       </c>
       <c r="E5">
-        <v>0.76238300000000003</v>
+        <v>0.74016349999999997</v>
       </c>
       <c r="F5">
-        <v>0.79794833595658499</v>
+        <v>0.78373603855582896</v>
       </c>
       <c r="G5">
-        <v>0.72004275427456399</v>
+        <v>0.69536135060680704</v>
       </c>
       <c r="H5">
-        <v>0.89475729192142595</v>
+        <v>0.89784468723436395</v>
       </c>
       <c r="J5" t="s">
         <v>28</v>
       </c>
-      <c r="K5">
+      <c r="K5" t="e">
         <f>B7/B8</f>
-        <v>3.0129502822023979</v>
+        <v>#VALUE!</v>
       </c>
       <c r="P5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6">
-        <v>137.43163418769799</v>
+        <v>67.619788885116506</v>
       </c>
       <c r="C6">
-        <v>6.4462380409240696</v>
+        <v>3.2557280063629102</v>
       </c>
       <c r="D6">
-        <v>0.88066234573316804</v>
+        <v>0.864447089900652</v>
       </c>
       <c r="E6">
-        <v>0.76238275</v>
+        <v>0.74016349999999997</v>
       </c>
       <c r="F6">
-        <v>0.79794816632777599</v>
+        <v>0.78373594855669404</v>
       </c>
       <c r="G6">
-        <v>0.72004247802820898</v>
+        <v>0.69536149487271004</v>
       </c>
       <c r="H6">
-        <v>0.89475729192142595</v>
+        <v>0.89784421049018304</v>
       </c>
       <c r="J6" t="s">
         <v>29</v>
       </c>
       <c r="K6">
         <f>B9/B10</f>
-        <v>3.5850017154059146</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+        <v>4.6020944459388504</v>
+      </c>
+      <c r="P6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
       <c r="B7">
-        <v>53.475140810012803</v>
+        <v>540.45999789237896</v>
       </c>
       <c r="C7">
-        <v>0.11669802665710401</v>
+        <v>1.2428181171417201</v>
       </c>
       <c r="D7">
-        <v>0.76869002635554995</v>
+        <v>0.84655055508365695</v>
       </c>
       <c r="E7">
-        <v>0.62206499999999998</v>
+        <v>0.70275874999999999</v>
       </c>
       <c r="F7">
-        <v>0.72133342033944903</v>
+        <v>0.76382006174231198</v>
       </c>
       <c r="G7">
-        <v>0.58803129822726496</v>
+        <v>0.65470266853913395</v>
       </c>
       <c r="H7">
-        <v>0.93278955892105098</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+        <v>0.91658454748157503</v>
+      </c>
+      <c r="P7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
-      <c r="B8">
-        <v>17.748431205749501</v>
-      </c>
-      <c r="C8">
-        <v>7.7227115631103502E-2</v>
-      </c>
-      <c r="D8">
-        <v>0.76370424960665395</v>
-      </c>
-      <c r="E8">
-        <v>0.62094724999999995</v>
-      </c>
-      <c r="F8">
-        <v>0.72077839685385303</v>
-      </c>
-      <c r="G8">
-        <v>0.58722236925571603</v>
-      </c>
-      <c r="H8">
-        <v>0.93297024496546199</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" t="s">
+        <v>17</v>
+      </c>
+      <c r="P8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
       <c r="B9">
-        <v>16.831475973129201</v>
+        <v>105.004899024963</v>
       </c>
       <c r="C9">
-        <v>0.189523935317993</v>
+        <v>1.16814589500427</v>
       </c>
       <c r="D9">
-        <v>0.76791211226968403</v>
+        <v>0.84561288598680395</v>
       </c>
       <c r="E9">
-        <v>0.62141349999999995</v>
+        <v>0.70202874999999998</v>
       </c>
       <c r="F9">
-        <v>0.72106663031906004</v>
+        <v>0.76337079066598201</v>
       </c>
       <c r="G9">
-        <v>0.58753041798901895</v>
+        <v>0.65405954337153804</v>
       </c>
       <c r="H9">
-        <v>0.93315855891676003</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+        <v>0.91655165213311995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
       <c r="B10">
-        <v>4.6949701309204102</v>
+        <v>22.816763162612901</v>
       </c>
       <c r="C10">
-        <v>7.6045036315917899E-2</v>
+        <v>0.15872502326965299</v>
       </c>
       <c r="D10">
-        <v>0.76501320933123595</v>
+        <v>0.84546133064648599</v>
       </c>
       <c r="E10">
-        <v>0.61808275000000001</v>
+        <v>0.70681349999999998</v>
       </c>
       <c r="F10">
-        <v>0.72018946252098304</v>
+        <v>0.76563547924235698</v>
       </c>
       <c r="G10">
-        <v>0.58475253815033101</v>
+        <v>0.65910089496242497</v>
       </c>
       <c r="H10">
-        <v>0.93727572165958395</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
+        <v>0.91324972193895604</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
@@ -815,30 +842,30 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
       <c r="B12">
-        <v>247.051288127899</v>
+        <v>244.96644806861801</v>
       </c>
       <c r="C12">
-        <v>14.5724880695343</v>
+        <v>15.346307992935101</v>
       </c>
       <c r="D12">
-        <v>0.50886502362989405</v>
+        <v>0.5</v>
       </c>
       <c r="E12">
-        <v>0.99423119833248896</v>
+        <v>0.99418766020669702</v>
       </c>
       <c r="F12">
-        <v>3.4608378870673903E-2</v>
+        <v>0</v>
       </c>
       <c r="G12">
-        <v>0.63333333333333297</v>
+        <v>0</v>
       </c>
       <c r="H12">
-        <v>1.7790262172284601E-2</v>
+        <v>0</v>
       </c>
       <c r="J12" t="s">
         <v>26</v>
@@ -848,7 +875,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -878,180 +905,180 @@
       </c>
       <c r="K13">
         <f>B14/B15</f>
-        <v>1.2545522987277054</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+        <v>1.1441141799606207</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
       <c r="B14">
-        <v>107.703871965408</v>
+        <v>70.201375961303697</v>
       </c>
       <c r="C14">
-        <v>2.4672060012817298</v>
+        <v>1.93897485733032</v>
       </c>
       <c r="D14">
-        <v>0.70216410847598598</v>
+        <v>0.71730578327843098</v>
       </c>
       <c r="E14">
-        <v>0.99431827458407396</v>
+        <v>0.994345485912695</v>
       </c>
       <c r="F14">
-        <v>0.16077170418006401</v>
+        <v>0.14203137902559801</v>
       </c>
       <c r="G14">
-        <v>0.56818181818181801</v>
+        <v>0.60139860139860102</v>
       </c>
       <c r="H14">
-        <v>9.3632958801498106E-2</v>
+        <v>8.0524344569288295E-2</v>
       </c>
       <c r="J14" t="s">
         <v>28</v>
       </c>
-      <c r="K14">
+      <c r="K14" t="e">
         <f>B16/B17</f>
-        <v>1.3576462016301398</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
       <c r="B15">
-        <v>85.850444078445406</v>
+        <v>61.358715057372997</v>
       </c>
       <c r="C15">
-        <v>2.19157791137695</v>
+        <v>1.74326395988464</v>
       </c>
       <c r="D15">
-        <v>0.70416710259434001</v>
+        <v>0.71708436738657799</v>
       </c>
       <c r="E15">
-        <v>0.99426929419255805</v>
+        <v>0.99428562098972995</v>
       </c>
       <c r="F15">
-        <v>0.145985401459854</v>
+        <v>0.136513157894736</v>
       </c>
       <c r="G15">
-        <v>0.54545454545454497</v>
+        <v>0.56081081081080997</v>
       </c>
       <c r="H15">
-        <v>8.4269662921348298E-2</v>
+        <v>7.77153558052434E-2</v>
       </c>
       <c r="J15" t="s">
         <v>29</v>
       </c>
       <c r="K15">
         <f>B18/B19</f>
-        <v>2.7881873746090426</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+        <v>2.5047971669251745</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
       <c r="B16">
-        <v>10.0587439537048</v>
+        <v>140.671549081802</v>
       </c>
       <c r="C16">
-        <v>2.54311561584472E-2</v>
+        <v>7.9900026321411105E-2</v>
       </c>
       <c r="D16">
-        <v>0.65589226445036397</v>
+        <v>0.70108406883378405</v>
       </c>
       <c r="E16">
-        <v>0.99427473645828202</v>
+        <v>0.99425840966111001</v>
       </c>
       <c r="F16">
-        <v>0.120401337792642</v>
+        <v>0.11715481171548101</v>
       </c>
       <c r="G16">
-        <v>0.5625</v>
+        <v>0.55118110236220397</v>
       </c>
       <c r="H16">
-        <v>6.7415730337078594E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+        <v>6.5543071161048599E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
-      <c r="B17">
-        <v>7.4089581966400102</v>
-      </c>
-      <c r="C17">
-        <v>5.2921056747436503E-2</v>
-      </c>
-      <c r="D17">
-        <v>0.656509208463391</v>
-      </c>
-      <c r="E17">
-        <v>0.99430194778690195</v>
-      </c>
-      <c r="F17">
-        <v>0.12531328320801999</v>
-      </c>
-      <c r="G17">
-        <v>0.581395348837209</v>
-      </c>
-      <c r="H17">
-        <v>7.02247191011236E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
       <c r="B18">
-        <v>12.824243068695001</v>
+        <v>74.015393972396794</v>
       </c>
       <c r="C18">
-        <v>1.1240959167480399E-2</v>
+        <v>6.4553022384643499E-2</v>
       </c>
       <c r="D18">
-        <v>0.65377386097916401</v>
+        <v>0.70360105525147698</v>
       </c>
       <c r="E18">
-        <v>0.99427473645828202</v>
+        <v>0.99430739005262603</v>
       </c>
       <c r="F18">
-        <v>0.121869782971619</v>
+        <v>0.12978369384359401</v>
       </c>
       <c r="G18">
-        <v>0.56153846153846099</v>
+        <v>0.58208955223880599</v>
       </c>
       <c r="H18">
-        <v>6.8352059925093606E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+        <v>7.3033707865168496E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>15</v>
       </c>
       <c r="B19">
-        <v>4.5994911193847603</v>
+        <v>29.5494561195373</v>
       </c>
       <c r="C19">
-        <v>5.2580118179321199E-2</v>
+        <v>0.33221912384033198</v>
       </c>
       <c r="D19">
-        <v>0.65627646255246397</v>
+        <v>0.71516730816973195</v>
       </c>
       <c r="E19">
-        <v>0.99428562098972995</v>
+        <v>0.994345485912695</v>
       </c>
       <c r="F19">
-        <v>0.126455906821963</v>
+        <v>0.12908633696563199</v>
       </c>
       <c r="G19">
-        <v>0.56716417910447703</v>
+        <v>0.61599999999999999</v>
       </c>
       <c r="H19">
-        <v>7.1161048689138501E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+        <v>7.2097378277153498E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -1077,243 +1104,243 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>8</v>
       </c>
       <c r="B21">
-        <v>8.9595470428466797</v>
+        <v>4.2575268745422301</v>
       </c>
       <c r="C21">
-        <v>1.64000988006591E-2</v>
+        <v>1.45189762115478E-2</v>
       </c>
       <c r="D21" t="s">
         <v>17</v>
       </c>
       <c r="E21">
-        <v>0.480050825921219</v>
+        <v>0.480559085133418</v>
       </c>
       <c r="F21">
-        <v>0.41735191279725298</v>
+        <v>0.41753640437300898</v>
       </c>
       <c r="G21">
-        <v>0.405571074996457</v>
+        <v>0.41276695117293699</v>
       </c>
       <c r="H21">
-        <v>0.480050825921219</v>
+        <v>0.480559085133418</v>
       </c>
       <c r="J21" t="s">
         <v>26</v>
       </c>
       <c r="K21">
         <f>B21/B22</f>
-        <v>1.3364487091426123</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+        <v>1.0493544459066011</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>9</v>
       </c>
       <c r="B22">
-        <v>6.70399618148803</v>
+        <v>4.0572819709777797</v>
       </c>
       <c r="C22">
-        <v>1.7077922821044901E-2</v>
+        <v>1.4071941375732399E-2</v>
       </c>
       <c r="D22" t="s">
         <v>17</v>
       </c>
       <c r="E22">
-        <v>0.47522236340533602</v>
+        <v>0.47115628970775097</v>
       </c>
       <c r="F22">
-        <v>0.41238316652260398</v>
+        <v>0.40864373814819699</v>
       </c>
       <c r="G22">
-        <v>0.40593742252221798</v>
+        <v>0.40542552287258199</v>
       </c>
       <c r="H22">
-        <v>0.47522236340533602</v>
+        <v>0.47115628970775097</v>
       </c>
       <c r="J22" t="s">
         <v>27</v>
       </c>
       <c r="K22">
         <f>B23/B24</f>
-        <v>0.38348280508029436</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+        <v>0.23447762998958924</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>10</v>
       </c>
       <c r="B23">
-        <v>0.78357696533203103</v>
+        <v>0.40218496322631803</v>
       </c>
       <c r="C23">
-        <v>8.7640285491943307E-3</v>
+        <v>6.3321590423583898E-3</v>
       </c>
       <c r="D23" t="s">
         <v>17</v>
       </c>
       <c r="E23">
-        <v>0.53418043202033005</v>
+        <v>0.53748411689961795</v>
       </c>
       <c r="F23">
-        <v>0.47213080520922102</v>
+        <v>0.46275790203997502</v>
       </c>
       <c r="G23">
-        <v>0.48882691136846201</v>
+        <v>0.48948241635230699</v>
       </c>
       <c r="H23">
-        <v>0.53418043202033005</v>
+        <v>0.53748411689961795</v>
       </c>
       <c r="J23" t="s">
         <v>28</v>
       </c>
       <c r="K23">
         <f>B25/B26</f>
-        <v>0.13061003861003889</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+        <v>0.64985153239002713</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>11</v>
       </c>
       <c r="B24">
-        <v>2.0433170795440598</v>
+        <v>1.71523809432983</v>
       </c>
       <c r="C24">
-        <v>1.04420185089111E-2</v>
+        <v>9.8171234130859306E-3</v>
       </c>
       <c r="D24" t="s">
         <v>17</v>
       </c>
       <c r="E24">
-        <v>0.53418043202033005</v>
+        <v>0.53748411689961795</v>
       </c>
       <c r="F24">
-        <v>0.47208385069553999</v>
+        <v>0.46275790203997502</v>
       </c>
       <c r="G24">
-        <v>0.48928940534741899</v>
+        <v>0.48948241635230699</v>
       </c>
       <c r="H24">
-        <v>0.53418043202033005</v>
+        <v>0.53748411689961795</v>
       </c>
       <c r="J24" t="s">
         <v>29</v>
       </c>
       <c r="K24">
         <f>B27/B28</f>
-        <v>0.44651313984168806</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+        <v>1.2568836980255964</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>12</v>
       </c>
       <c r="B25">
-        <v>4.6375036239624003E-2</v>
+        <v>0.77965283393859797</v>
       </c>
       <c r="C25">
-        <v>2.42948532104492E-4</v>
+        <v>2.3519992828369102E-3</v>
       </c>
       <c r="D25" t="s">
         <v>17</v>
       </c>
       <c r="E25">
-        <v>0.53875476493011398</v>
+        <v>0.54129606099110505</v>
       </c>
       <c r="F25">
-        <v>0.45513594678653801</v>
+        <v>0.46549872521500602</v>
       </c>
       <c r="G25">
-        <v>0.399598203951259</v>
+        <v>0.49836879790121602</v>
       </c>
       <c r="H25">
-        <v>0.53875476493011398</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+        <v>0.54129606099110505</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>13</v>
       </c>
       <c r="B26">
-        <v>0.35506486892700101</v>
+        <v>1.19973993301391</v>
       </c>
       <c r="C26">
-        <v>2.4628639221191402E-3</v>
+        <v>3.3330917358398398E-3</v>
       </c>
       <c r="D26" t="s">
         <v>17</v>
       </c>
       <c r="E26">
-        <v>0.53875476493011398</v>
+        <v>0.54129606099110505</v>
       </c>
       <c r="F26">
-        <v>0.45513594678653801</v>
+        <v>0.46384763520248401</v>
       </c>
       <c r="G26">
-        <v>0.399598203951259</v>
+        <v>0.49281387720424802</v>
       </c>
       <c r="H26">
-        <v>0.53875476493011398</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+        <v>0.54129606099110505</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>14</v>
       </c>
       <c r="B27">
-        <v>0.12608504295349099</v>
+        <v>1.6472580432891799</v>
       </c>
       <c r="C27">
-        <v>2.7298927307128901E-4</v>
+        <v>2.3999214172363199E-3</v>
       </c>
       <c r="D27" t="s">
         <v>17</v>
       </c>
       <c r="E27">
-        <v>0.53926302414231198</v>
+        <v>0.53748411689961795</v>
       </c>
       <c r="F27">
-        <v>0.45534595816103501</v>
+        <v>0.462144650384823</v>
       </c>
       <c r="G27">
-        <v>0.39993619592850499</v>
+        <v>0.48170437730093602</v>
       </c>
       <c r="H27">
-        <v>0.53926302414231198</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+        <v>0.53748411689961795</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>15</v>
       </c>
       <c r="B28">
-        <v>0.28237700462341297</v>
+        <v>1.3105890750885001</v>
       </c>
       <c r="C28">
-        <v>1.0204076766967701E-2</v>
+        <v>6.7760944366455E-3</v>
       </c>
       <c r="D28" t="s">
         <v>17</v>
       </c>
       <c r="E28">
-        <v>0.53926302414231198</v>
+        <v>0.54053367217280801</v>
       </c>
       <c r="F28">
-        <v>0.45534595816103501</v>
+        <v>0.46571787206051901</v>
       </c>
       <c r="G28">
-        <v>0.39993619592850499</v>
+        <v>0.50074868935259698</v>
       </c>
       <c r="H28">
-        <v>0.53926302414231198</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+        <v>0.54053367217280801</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>19</v>
       </c>
@@ -1339,48 +1366,48 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>8</v>
       </c>
       <c r="B30">
-        <v>10.4681220054626</v>
+        <v>9.6328449249267507</v>
       </c>
       <c r="C30">
-        <v>0.19880414009094199</v>
+        <v>0.196533918380737</v>
       </c>
       <c r="D30">
-        <v>0.864817968798272</v>
+        <v>0.86821393320162299</v>
       </c>
       <c r="E30">
-        <v>0.99943822197254295</v>
+        <v>0.99948503680816403</v>
       </c>
       <c r="F30">
-        <v>0.81818181818181801</v>
+        <v>0.83206106870229002</v>
       </c>
       <c r="G30">
-        <v>0.93103448275862</v>
+        <v>0.95614035087719296</v>
       </c>
       <c r="H30">
-        <v>0.72972972972972905</v>
+        <v>0.73648648648648596</v>
       </c>
       <c r="J30" t="s">
         <v>26</v>
       </c>
       <c r="K30">
         <f>B30/B31</f>
-        <v>1.4878503450438723</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+        <v>1.3455285765819138</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>9</v>
       </c>
       <c r="B31">
-        <v>7.0357358455657897</v>
+        <v>7.1591529846191397</v>
       </c>
       <c r="C31">
-        <v>0.19870591163635201</v>
+        <v>0.204784154891967</v>
       </c>
       <c r="D31">
         <v>0.874947241925083</v>
@@ -1402,18 +1429,18 @@
       </c>
       <c r="K31">
         <f>B32/B33</f>
-        <v>0.34597503659130119</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+        <v>0.35125462866502499</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>10</v>
       </c>
       <c r="B32">
-        <v>0.41484308242797802</v>
+        <v>0.428867816925048</v>
       </c>
       <c r="C32">
-        <v>1.6106128692626901E-2</v>
+        <v>1.6045808792114199E-2</v>
       </c>
       <c r="D32">
         <v>0.96703151067123105</v>
@@ -1435,18 +1462,18 @@
       </c>
       <c r="K32">
         <f>B34/B35</f>
-        <v>0.4289028947249191</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+        <v>1.4613502230129545</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>11</v>
       </c>
       <c r="B33">
-        <v>1.1990549564361499</v>
+        <v>1.2209599018096899</v>
       </c>
       <c r="C33">
-        <v>1.5221834182739201E-2</v>
+        <v>1.60748958587646E-2</v>
       </c>
       <c r="D33">
         <v>0.96703166910388805</v>
@@ -1468,114 +1495,114 @@
       </c>
       <c r="K33">
         <f>B36/B37</f>
-        <v>0.95366493750977444</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+        <v>1.9459128409324746</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>12</v>
       </c>
       <c r="B34">
-        <v>0.21440982818603499</v>
+        <v>1.9117078781127901</v>
       </c>
       <c r="C34">
-        <v>8.2087516784667904E-4</v>
+        <v>5.2549839019775304E-3</v>
       </c>
       <c r="D34">
-        <v>0.90857263265962396</v>
+        <v>0.95517635139095902</v>
       </c>
       <c r="E34">
-        <v>0.99919244408552998</v>
+        <v>0.99936799971910995</v>
       </c>
       <c r="F34">
-        <v>0.75789473684210495</v>
+        <v>0.80985915492957705</v>
       </c>
       <c r="G34">
-        <v>0.78832116788321105</v>
+        <v>0.84558823529411697</v>
       </c>
       <c r="H34">
-        <v>0.72972972972972905</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+        <v>0.77702702702702697</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>13</v>
       </c>
       <c r="B35">
-        <v>0.499902963638305</v>
+        <v>1.3081791400909399</v>
       </c>
       <c r="C35">
-        <v>5.7318210601806597E-3</v>
+        <v>7.3399543762206997E-3</v>
       </c>
       <c r="D35">
-        <v>0.90856257218587899</v>
+        <v>0.96889947131022203</v>
       </c>
       <c r="E35">
-        <v>0.99926266633896199</v>
+        <v>0.99941481455473202</v>
       </c>
       <c r="F35">
-        <v>0.78929765886287595</v>
+        <v>0.82269503546099199</v>
       </c>
       <c r="G35">
-        <v>0.78145695364238399</v>
+        <v>0.86567164179104406</v>
       </c>
       <c r="H35">
-        <v>0.79729729729729704</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+        <v>0.78378378378378299</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>14</v>
       </c>
       <c r="B36">
-        <v>0.248564958572387</v>
+        <v>1.0934898853302</v>
       </c>
       <c r="C36">
-        <v>8.5496902465820302E-4</v>
+        <v>7.9159736633300695E-3</v>
       </c>
       <c r="D36">
-        <v>0.91901172084799498</v>
+        <v>0.965868852614851</v>
       </c>
       <c r="E36">
-        <v>0.99921585150334102</v>
+        <v>0.99930948117458396</v>
       </c>
       <c r="F36">
-        <v>0.77288135593220297</v>
+        <v>0.79442508710801296</v>
       </c>
       <c r="G36">
-        <v>0.77551020408163196</v>
+        <v>0.82014388489208601</v>
       </c>
       <c r="H36">
         <v>0.77027027027026995</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>15</v>
       </c>
       <c r="B37">
-        <v>0.26064181327819802</v>
+        <v>0.56194186210632302</v>
       </c>
       <c r="C37">
-        <v>5.7289600372314401E-3</v>
+        <v>7.17687606811523E-3</v>
       </c>
       <c r="D37">
-        <v>0.91179974745834402</v>
+        <v>0.96353208974259397</v>
       </c>
       <c r="E37">
-        <v>0.99927437004786801</v>
+        <v>0.99939140713692098</v>
       </c>
       <c r="F37">
-        <v>0.78911564625850295</v>
+        <v>0.81294964028776895</v>
       </c>
       <c r="G37">
-        <v>0.79452054794520499</v>
+        <v>0.86923076923076903</v>
       </c>
       <c r="H37">
-        <v>0.78378378378378299</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+        <v>0.76351351351351304</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>20</v>
       </c>
@@ -1601,63 +1628,63 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>8</v>
       </c>
       <c r="B39">
-        <v>387.49875903129498</v>
+        <v>244.28486108779899</v>
       </c>
       <c r="C39">
-        <v>1.5469288825988701</v>
+        <v>1.3483309745788501</v>
       </c>
       <c r="D39">
-        <v>0.72446914164882603</v>
+        <v>0.71646244739306297</v>
       </c>
       <c r="E39">
-        <v>0.72596799999999995</v>
+        <v>0.71802600000000005</v>
       </c>
       <c r="F39">
-        <v>0.74351179333582895</v>
+        <v>0.73622687328929204</v>
       </c>
       <c r="G39">
-        <v>0.73760213935522201</v>
+        <v>0.72997057961497502</v>
       </c>
       <c r="H39">
-        <v>0.74951690821256001</v>
+        <v>0.74259133454106196</v>
       </c>
       <c r="J39" t="s">
         <v>26</v>
       </c>
       <c r="K39">
         <f>B39/B40</f>
-        <v>3.2193643922713395</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+        <v>2.7776717201747716</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>9</v>
       </c>
       <c r="B40">
-        <v>120.364988803863</v>
+        <v>87.945907831192002</v>
       </c>
       <c r="C40">
-        <v>1.8243761062621999</v>
+        <v>1.4156398773193299</v>
       </c>
       <c r="D40">
-        <v>0.72475025193573706</v>
+        <v>0.71651312100643505</v>
       </c>
       <c r="E40">
-        <v>0.72624200000000005</v>
+        <v>0.71809599999999996</v>
       </c>
       <c r="F40">
-        <v>0.74374378684599196</v>
+        <v>0.736372749988778</v>
       </c>
       <c r="G40">
-        <v>0.73790162302322904</v>
+        <v>0.72989647910301603</v>
       </c>
       <c r="H40">
-        <v>0.74967919685990303</v>
+        <v>0.74296497584540999</v>
       </c>
       <c r="J40" t="s">
         <v>27</v>
@@ -1667,30 +1694,30 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>10</v>
       </c>
       <c r="B41">
-        <v>128.355188131332</v>
+        <v>86.059884071350098</v>
       </c>
       <c r="C41">
-        <v>0.56760501861572199</v>
+        <v>0.29416084289550698</v>
       </c>
       <c r="D41">
-        <v>0.82058667428228804</v>
+        <v>0.81275250797903498</v>
       </c>
       <c r="E41">
-        <v>0.70701400000000003</v>
+        <v>0.69657800000000003</v>
       </c>
       <c r="F41">
-        <v>0.76764366731327704</v>
+        <v>0.76205368695938502</v>
       </c>
       <c r="G41">
-        <v>0.66205845578880795</v>
+        <v>0.651961086883596</v>
       </c>
       <c r="H41">
-        <v>0.91329634661835701</v>
+        <v>0.91688179347826004</v>
       </c>
       <c r="J41" t="s">
         <v>28</v>
@@ -1700,7 +1727,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>11</v>
       </c>
@@ -1730,10 +1757,10 @@
       </c>
       <c r="K42">
         <f>B45/B46</f>
-        <v>2.4435968423133501</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+        <v>4.0736947903615164</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>12</v>
       </c>
@@ -1759,7 +1786,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>13</v>
       </c>
@@ -1785,59 +1812,59 @@
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>14</v>
       </c>
       <c r="B45">
-        <v>12.513502836227399</v>
+        <v>58.499768018722499</v>
       </c>
       <c r="C45">
-        <v>2.0787954330444301E-2</v>
+        <v>8.6911916732788003E-2</v>
       </c>
       <c r="D45">
-        <v>0.75770072351590401</v>
+        <v>0.80570472140444505</v>
       </c>
       <c r="E45">
-        <v>0.62521400000000005</v>
+        <v>0.68078000000000005</v>
       </c>
       <c r="F45">
-        <v>0.72860120120902905</v>
+        <v>0.75513328751319297</v>
       </c>
       <c r="G45">
-        <v>0.59114570481139095</v>
+        <v>0.63615896025476604</v>
       </c>
       <c r="H45">
-        <v>0.94934707125603801</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+        <v>0.92884586352656995</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>15</v>
       </c>
       <c r="B46">
-        <v>5.1209359169006303</v>
+        <v>14.3603708744049</v>
       </c>
       <c r="C46">
-        <v>2.1116018295287999E-2</v>
+        <v>3.5959005355834898E-2</v>
       </c>
       <c r="D46">
-        <v>0.75667458095033602</v>
+        <v>0.806738224269964</v>
       </c>
       <c r="E46">
-        <v>0.62407800000000002</v>
+        <v>0.686338</v>
       </c>
       <c r="F46">
-        <v>0.72791964436930101</v>
+        <v>0.75713469391547505</v>
       </c>
       <c r="G46">
-        <v>0.59040221288706096</v>
+        <v>0.641978712843986</v>
       </c>
       <c r="H46">
-        <v>0.94895078502415398</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+        <v>0.92263360507246295</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>21</v>
       </c>
@@ -1863,81 +1890,81 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>8</v>
       </c>
       <c r="B48">
-        <v>57.0858249664306</v>
+        <v>53.730160951614302</v>
       </c>
       <c r="C48">
-        <v>2.5925111770629798</v>
+        <v>2.29514288902282</v>
       </c>
       <c r="D48" t="s">
         <v>17</v>
       </c>
       <c r="E48">
-        <v>0.54991307452637295</v>
+        <v>0.55052091524659996</v>
       </c>
       <c r="F48">
-        <v>0.51037711797889296</v>
+        <v>0.51063744663122801</v>
       </c>
       <c r="G48">
-        <v>0.484392763368164</v>
+        <v>0.48356099117343498</v>
       </c>
       <c r="H48">
-        <v>0.54991307452637295</v>
+        <v>0.55052091524659996</v>
       </c>
       <c r="J48" t="s">
         <v>26</v>
       </c>
       <c r="K48">
         <f>B48/B49</f>
-        <v>2.0584834846833546</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+        <v>1.9431228005260242</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>9</v>
       </c>
       <c r="B49">
-        <v>27.731981039047199</v>
+        <v>27.6514489650726</v>
       </c>
       <c r="C49">
-        <v>2.6190509796142498</v>
+        <v>2.37886214256286</v>
       </c>
       <c r="D49" t="s">
         <v>17</v>
       </c>
       <c r="E49">
-        <v>0.54912670716104295</v>
+        <v>0.54834459043012096</v>
       </c>
       <c r="F49">
-        <v>0.50971545349787195</v>
+        <v>0.50896802325010204</v>
       </c>
       <c r="G49">
-        <v>0.48407958153006603</v>
+        <v>0.483186929998564</v>
       </c>
       <c r="H49">
-        <v>0.54912670716104295</v>
+        <v>0.54834459043012096</v>
       </c>
       <c r="J49" t="s">
         <v>27</v>
       </c>
       <c r="K49">
         <f>B50/B51</f>
-        <v>0.76350343522039266</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+        <v>0.79313257107344903</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>10</v>
       </c>
       <c r="B50">
-        <v>41.048416137695298</v>
+        <v>40.609479904174798</v>
       </c>
       <c r="C50">
-        <v>0.89361810684204102</v>
+        <v>0.88867998123168901</v>
       </c>
       <c r="D50" t="s">
         <v>17</v>
@@ -1959,147 +1986,147 @@
       </c>
       <c r="K50">
         <f>B52/B53</f>
-        <v>1.2946957275400519</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+        <v>1.4153099191772547</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>11</v>
       </c>
       <c r="B51">
-        <v>53.763236999511697</v>
+        <v>51.201377153396599</v>
       </c>
       <c r="C51">
-        <v>0.88830614089965798</v>
+        <v>0.88277316093444802</v>
       </c>
       <c r="D51" t="s">
         <v>17</v>
       </c>
       <c r="E51">
-        <v>0.56835657721915001</v>
+        <v>0.56774448586451498</v>
       </c>
       <c r="F51">
-        <v>0.53150509455672301</v>
+        <v>0.53123215859804895</v>
       </c>
       <c r="G51">
-        <v>0.53970691876870702</v>
+        <v>0.53920459205646698</v>
       </c>
       <c r="H51">
-        <v>0.56835657721915001</v>
+        <v>0.56774448586451498</v>
       </c>
       <c r="J51" t="s">
         <v>29</v>
       </c>
       <c r="K51">
         <f>B54/B55</f>
-        <v>7.8878572050112528</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+        <v>8.8158158703353102</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>12</v>
       </c>
       <c r="B52">
-        <v>24.483930110931301</v>
+        <v>233.17652106284999</v>
       </c>
       <c r="C52">
-        <v>9.5459222793579102E-2</v>
+        <v>0.60153222084045399</v>
       </c>
       <c r="D52" t="s">
         <v>17</v>
       </c>
       <c r="E52">
-        <v>0.56278399551132996</v>
+        <v>0.56819930374608396</v>
       </c>
       <c r="F52">
-        <v>0.51553680725175</v>
+        <v>0.52982353679646399</v>
       </c>
       <c r="G52">
-        <v>0.53636747542815499</v>
+        <v>0.53988811351919797</v>
       </c>
       <c r="H52">
-        <v>0.56278399551132996</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+        <v>0.56819930374608396</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>13</v>
       </c>
       <c r="B53">
-        <v>18.910953044891301</v>
+        <v>164.752975940704</v>
       </c>
       <c r="C53">
-        <v>0.20873284339904699</v>
+        <v>1.43372702598571</v>
       </c>
       <c r="D53" t="s">
         <v>17</v>
       </c>
       <c r="E53">
-        <v>0.56263522330707805</v>
+        <v>0.56744694145601204</v>
       </c>
       <c r="F53">
-        <v>0.51507546331440501</v>
+        <v>0.52894419417011396</v>
       </c>
       <c r="G53">
-        <v>0.53555932854176502</v>
+        <v>0.53908305765770304</v>
       </c>
       <c r="H53">
-        <v>0.56263522330707805</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+        <v>0.56744694145601204</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>14</v>
       </c>
       <c r="B54">
-        <v>31.2297859191894</v>
+        <v>230.15626096725401</v>
       </c>
       <c r="C54">
-        <v>6.2227010726928697E-2</v>
+        <v>0.569161176681518</v>
       </c>
       <c r="D54" t="s">
         <v>17</v>
       </c>
       <c r="E54">
-        <v>0.56263097267267104</v>
+        <v>0.56795701758487405</v>
       </c>
       <c r="F54">
-        <v>0.51524776024387497</v>
+        <v>0.52987988210048298</v>
       </c>
       <c r="G54">
-        <v>0.53499668644968201</v>
+        <v>0.53878050784568199</v>
       </c>
       <c r="H54">
-        <v>0.56263097267267104</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
+        <v>0.56795701758487405</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>15</v>
       </c>
       <c r="B55">
-        <v>3.9592230319976802</v>
+        <v>26.107199192047101</v>
       </c>
       <c r="C55">
-        <v>0.196581125259399</v>
+        <v>1.4060571193695</v>
       </c>
       <c r="D55" t="s">
         <v>17</v>
       </c>
       <c r="E55">
-        <v>0.562941268984395</v>
+        <v>0.56853510386425099</v>
       </c>
       <c r="F55">
-        <v>0.51576653150531904</v>
+        <v>0.53040334971192105</v>
       </c>
       <c r="G55">
-        <v>0.53650275349126997</v>
+        <v>0.53976928261546597</v>
       </c>
       <c r="H55">
-        <v>0.562941268984395</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+        <v>0.56853510386425099</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>22</v>
       </c>
@@ -2125,48 +2152,48 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>8</v>
       </c>
       <c r="B57">
-        <v>185.37674403190599</v>
+        <v>180.19692587852401</v>
       </c>
       <c r="C57">
-        <v>8.5752570629119802</v>
+        <v>8.1206378936767507</v>
       </c>
       <c r="D57" t="s">
         <v>17</v>
       </c>
       <c r="E57">
-        <v>0.55514454951567005</v>
+        <v>0.55519941971419295</v>
       </c>
       <c r="F57">
-        <v>0.51565251792972799</v>
+        <v>0.51573261889564104</v>
       </c>
       <c r="G57">
-        <v>0.49212363086090499</v>
+        <v>0.49233004449838003</v>
       </c>
       <c r="H57">
-        <v>0.55514454951567005</v>
+        <v>0.55519941971419295</v>
       </c>
       <c r="J57" t="s">
         <v>26</v>
       </c>
       <c r="K57">
         <f>B57/B58</f>
-        <v>2.9602234076081153</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
+        <v>2.8586284440276275</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>9</v>
       </c>
       <c r="B58">
-        <v>62.6225519180297</v>
+        <v>63.036148071288999</v>
       </c>
       <c r="C58">
-        <v>8.3687090873718208</v>
+        <v>8.0460729598999006</v>
       </c>
       <c r="D58" t="s">
         <v>17</v>
@@ -2188,18 +2215,18 @@
       </c>
       <c r="K58">
         <f>B59/B60</f>
-        <v>1.2659168606108411</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
+        <v>1.2758380735360466</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>10</v>
       </c>
       <c r="B59">
-        <v>118.024870872497</v>
+        <v>119.648628950119</v>
       </c>
       <c r="C59">
-        <v>2.84838795661926</v>
+        <v>2.68793392181396</v>
       </c>
       <c r="D59" t="s">
         <v>17</v>
@@ -2224,66 +2251,66 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>11</v>
       </c>
       <c r="B60">
-        <v>93.232718944549504</v>
+        <v>93.780418872833195</v>
       </c>
       <c r="C60">
-        <v>2.7960948944091699</v>
+        <v>2.7575352191925</v>
       </c>
       <c r="D60" t="s">
         <v>17</v>
       </c>
       <c r="E60">
-        <v>0.57525246982808198</v>
+        <v>0.57522838047263303</v>
       </c>
       <c r="F60">
-        <v>0.54028636680086894</v>
+        <v>0.54049064658851897</v>
       </c>
       <c r="G60">
-        <v>0.55077486937908504</v>
+        <v>0.55103383940185202</v>
       </c>
       <c r="H60">
-        <v>0.57525246982808198</v>
+        <v>0.57522838047263303</v>
       </c>
       <c r="J60" t="s">
         <v>29</v>
       </c>
       <c r="K60">
         <f>B63/B64</f>
-        <v>4.3218633188934383</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
+        <v>5.0850574422263284</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>12</v>
       </c>
       <c r="B61">
-        <v>87.105005025863605</v>
+        <v>840.76587104797295</v>
       </c>
       <c r="C61">
-        <v>0.27959704399108798</v>
+        <v>1.75413393974304</v>
       </c>
       <c r="D61" t="s">
         <v>17</v>
       </c>
       <c r="E61">
-        <v>0.565895093533614</v>
+        <v>0.57380443190608299</v>
       </c>
       <c r="F61">
-        <v>0.52105112699948797</v>
+        <v>0.53738030433031003</v>
       </c>
       <c r="G61">
-        <v>0.54316799702640495</v>
+        <v>0.54984792738212096</v>
       </c>
       <c r="H61">
-        <v>0.565895093533614</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
+        <v>0.57380443190608299</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>13</v>
       </c>
@@ -2309,59 +2336,59 @@
         <v>17</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>14</v>
       </c>
       <c r="B63">
-        <v>52.247627973556497</v>
+        <v>391.30918908119202</v>
       </c>
       <c r="C63">
-        <v>0.176508903503417</v>
+        <v>1.6533501148223799</v>
       </c>
       <c r="D63" t="s">
         <v>17</v>
       </c>
       <c r="E63">
-        <v>0.56580408930191695</v>
+        <v>0.57437187005666301</v>
       </c>
       <c r="F63">
-        <v>0.52092424153397299</v>
+        <v>0.53837752021419305</v>
       </c>
       <c r="G63">
-        <v>0.54243033063211299</v>
+        <v>0.55064677322581101</v>
       </c>
       <c r="H63">
-        <v>0.56580408930191695</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
+        <v>0.57437187005666301</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>15</v>
       </c>
       <c r="B64">
-        <v>12.0891439914703</v>
+        <v>76.952756881713796</v>
       </c>
       <c r="C64">
-        <v>0.52948403358459395</v>
+        <v>4.3804979324340803</v>
       </c>
       <c r="D64" t="s">
         <v>17</v>
       </c>
       <c r="E64">
-        <v>0.56582416376479105</v>
+        <v>0.57459938063590499</v>
       </c>
       <c r="F64">
-        <v>0.52092701479679504</v>
+        <v>0.53836030055053297</v>
       </c>
       <c r="G64">
-        <v>0.54286977739970199</v>
+        <v>0.55092883524532199</v>
       </c>
       <c r="H64">
-        <v>0.56582416376479105</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+        <v>0.57459938063590499</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>23</v>
       </c>
@@ -2387,48 +2414,48 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>8</v>
       </c>
       <c r="B66">
-        <v>562.36591339111305</v>
+        <v>544.22584891319195</v>
       </c>
       <c r="C66">
-        <v>14.7402906417846</v>
+        <v>14.5915539264678</v>
       </c>
       <c r="D66" t="s">
         <v>17</v>
       </c>
       <c r="E66">
-        <v>0.59828435845957295</v>
+        <v>0.59846687351706496</v>
       </c>
       <c r="F66">
-        <v>0.88505420782296096</v>
+        <v>0.88480311540176404</v>
       </c>
       <c r="G66">
-        <v>0.92229334515335604</v>
+        <v>0.92279873803874501</v>
       </c>
       <c r="H66">
-        <v>0.86972705307711695</v>
+        <v>0.86882664546015498</v>
       </c>
       <c r="J66" t="s">
         <v>26</v>
       </c>
       <c r="K66">
         <f>B66/B67</f>
-        <v>0.74304427597489175</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
+        <v>0.73894995736746827</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>9</v>
       </c>
       <c r="B67">
-        <v>756.840381622314</v>
+        <v>736.48539185523896</v>
       </c>
       <c r="C67">
-        <v>13.8551008701324</v>
+        <v>13.6015799045562</v>
       </c>
       <c r="D67" t="s">
         <v>17</v>
@@ -2450,18 +2477,18 @@
       </c>
       <c r="K67">
         <f>B68/B69</f>
-        <v>0.3331119008154354</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
+        <v>0.32606470258984749</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>10</v>
       </c>
       <c r="B68">
-        <v>153.87739300727799</v>
+        <v>151.334974050521</v>
       </c>
       <c r="C68">
-        <v>0.54269909858703602</v>
+        <v>0.56721997261047297</v>
       </c>
       <c r="D68" t="s">
         <v>17</v>
@@ -2483,18 +2510,18 @@
       </c>
       <c r="K68">
         <f>B70/B71</f>
-        <v>0.77063246395884355</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
+        <v>1.085357948288296</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>11</v>
       </c>
       <c r="B69">
-        <v>461.93904399871798</v>
+        <v>464.12559485435401</v>
       </c>
       <c r="C69">
-        <v>0.63034319877624501</v>
+        <v>0.70114254951476995</v>
       </c>
       <c r="D69" t="s">
         <v>17</v>
@@ -2516,111 +2543,111 @@
       </c>
       <c r="K69">
         <f>B72/B73</f>
-        <v>8.6260649162468148</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
+        <v>15.825411412094915</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>12</v>
       </c>
       <c r="B70">
-        <v>43.073297739028902</v>
+        <v>201.87754178047101</v>
       </c>
       <c r="C70">
-        <v>7.2958707809448201E-2</v>
+        <v>6.27288818359375E-2</v>
       </c>
       <c r="D70" t="s">
         <v>17</v>
       </c>
       <c r="E70">
-        <v>0</v>
+        <v>0.34166818762547901</v>
       </c>
       <c r="F70">
-        <v>0.28337055044981202</v>
+        <v>0.80378698860495601</v>
       </c>
       <c r="G70">
-        <v>0.169223666834866</v>
+        <v>0.717244558588782</v>
       </c>
       <c r="H70">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
+        <v>0.97676626774089803</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>13</v>
       </c>
       <c r="B71">
-        <v>55.893437862396198</v>
+        <v>186.00088763237</v>
       </c>
       <c r="C71">
-        <v>0.25314664840698198</v>
+        <v>0.29358696937561002</v>
       </c>
       <c r="D71" t="s">
         <v>17</v>
       </c>
       <c r="E71">
-        <v>0</v>
+        <v>0.33692279613067999</v>
       </c>
       <c r="F71">
-        <v>0.283438020470208</v>
+        <v>0.80190365818995901</v>
       </c>
       <c r="G71">
-        <v>0.16927533470040601</v>
+        <v>0.714876136011379</v>
       </c>
       <c r="H71">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
+        <v>0.97643296048114403</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>14</v>
       </c>
       <c r="B72">
-        <v>432.17568826675398</v>
+        <v>1823.9185843467701</v>
       </c>
       <c r="C72">
-        <v>8.6051225662231404E-2</v>
+        <v>0.106192111968994</v>
       </c>
       <c r="D72" t="s">
         <v>17</v>
       </c>
       <c r="E72">
-        <v>0</v>
+        <v>0.33947800693557201</v>
       </c>
       <c r="F72">
-        <v>0.28337055044981202</v>
+        <v>0.80364455635812504</v>
       </c>
       <c r="G72">
-        <v>0.169223666834866</v>
+        <v>0.71715576356477895</v>
       </c>
       <c r="H72">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
+        <v>0.97693661512788998</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>15</v>
       </c>
       <c r="B73">
-        <v>50.101140260696397</v>
+        <v>115.252522468566</v>
       </c>
       <c r="C73">
-        <v>0.24238848686218201</v>
+        <v>0.28674292564392001</v>
       </c>
       <c r="D73" t="s">
         <v>17</v>
       </c>
       <c r="E73">
-        <v>0</v>
+        <v>0.342945793027924</v>
       </c>
       <c r="F73">
-        <v>0.28337055044981202</v>
+        <v>0.80348055718883304</v>
       </c>
       <c r="G73">
-        <v>0.169223666834866</v>
+        <v>0.717519957481629</v>
       </c>
       <c r="H73">
-        <v>1</v>
+        <v>0.976329100722238</v>
       </c>
     </row>
   </sheetData>

</xml_diff>